<commit_message>
sridevi folder in nico folder
</commit_message>
<xml_diff>
--- a/Nico C/To DO.xlsx
+++ b/Nico C/To DO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://corsair-my.sharepoint.com/personal/nico_cosereanu_corsair_com/Documents/Documents/Nico/Data Analytics Boot Camp/GT-VIRT-DATA-PT-09-2022-U-LOLC/Project-4/Nico C/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="8_{E14536B2-42AA-4FF7-89E9-942404F05D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBABDAB3-A944-40C6-A58A-00FFDCE2499E}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="8_{E14536B2-42AA-4FF7-89E9-942404F05D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E385FAE1-6889-4E95-82D6-B43A44C16798}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{121FE3AF-D380-4301-B961-78B46CBCC39D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>Who</t>
   </si>
@@ -150,9 +150,6 @@
   </si>
   <si>
     <t>done</t>
-  </si>
-  <si>
-    <t>wip</t>
   </si>
 </sst>
 </file>
@@ -531,7 +528,7 @@
   <dimension ref="C2:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,7 +577,7 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">

</xml_diff>